<commit_message>
update Fri Dec 15 18:02:46 EST 2017
</commit_message>
<xml_diff>
--- a/VISta timeline.xlsx
+++ b/VISta timeline.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="22060" windowWidth="33600" windowHeight="19500" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="10060" windowWidth="38400" windowHeight="10560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="112">
   <si>
     <t>Source table prep</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Task / Functionality of code needed</t>
-  </si>
-  <si>
-    <t>Template form still being designed</t>
   </si>
   <si>
     <t>gnomAD coverage file</t>
@@ -118,9 +115,6 @@
     <t>dbNSFP</t>
   </si>
   <si>
-    <t>Compare, assess, determine cutoffs for REVEL, CADD, metaSVM vs SIFT, PolyPhen2, MutationTaster2</t>
-  </si>
-  <si>
     <t>multiz100way</t>
   </si>
   <si>
@@ -159,30 +153,7 @@
     <t>Pathogenic variant database</t>
   </si>
   <si>
-    <t>Determine final fields to be used for joined pathogenic variant database (maintain # pts and refs)</t>
-  </si>
-  <si>
     <t>Predictions and computational</t>
-  </si>
-  <si>
-    <t>is_pos_covered
-I: Chromosomal position
-O: Is the position covered &gt; 20x/sample on average? (yes or no)</t>
-  </si>
-  <si>
-    <t>suggest_BS2
-I: VCF variant
-O: BS2 or other options</t>
-  </si>
-  <si>
-    <t>suggest_BA1_BS1_PM2
-I: VCF variant
-O: BA1, BS1, PM2, or other options</t>
-  </si>
-  <si>
-    <t>get_genotype_counts
-I: VCF variant
-O: genotype counts at this position (number homoz, hetero, hemiz)</t>
   </si>
   <si>
     <t>suggest_final_pathogenicity
@@ -196,11 +167,6 @@
 (if no transcript version, assume most current)</t>
   </si>
   <si>
-    <t>normalize_VCF
-I: VCF variant
-O: left-normalized VCF variant</t>
-  </si>
-  <si>
     <t>get_all_cdot_and_pdot
 I: VCF variant
 O: all possible HGVS c. and p. for all refGene NM_ and NR_ transcripts
@@ -213,19 +179,9 @@
 (discrepancies will trigger manual review and correction of the official disease transcript c. and p. in RVS db)</t>
   </si>
   <si>
-    <t xml:space="preserve">get_pathogenic_variants_MVL
-I: chr, start, stop
-O: Variants from pathogenic db with </t>
-  </si>
-  <si>
     <t>get_benign_variants
 I: chr, start, stop
 O: variants with MAF &gt; (5% or disease AF?), and variants with concordant Ben or LBen assertions</t>
-  </si>
-  <si>
-    <t>get_pathogenic_variants
-I: chr, start, stop
-O: Variants from pathogenic db with a pathogenic assertion (allow discordant for review purposes)</t>
   </si>
   <si>
     <t>suggest_BP3
@@ -251,21 +207,6 @@
 O: yes or no</t>
   </si>
   <si>
-    <t>suggest_PP5_BP6
-I: VCF variant, transcript
-O: PP5, BP6, or other options (concordant assertions, no publication references, not in MVL, compare get_patho to get_patho_MVL)</t>
-  </si>
-  <si>
-    <t>suggest_PS4
-I: VCF variant, transcript
-O: PS4-M, PS4-P, or other options</t>
-  </si>
-  <si>
-    <t>get_variant_type
-I: VCF variant, transcript
-O: variant type (stopgain, frameshift, CSS, stoploss, startloss, inframe, nonsynonymous, intronic)</t>
-  </si>
-  <si>
     <t>get_valid_disease_variant_types
 I: phenotype_ID, transcript
 O: missense only/LOF only/any</t>
@@ -309,11 +250,6 @@
   <si>
     <t>Overseeing manually curated disease-relevant transcript, disease allele frequency cutoff, inheritance pattern, can BS1 be applied (age of onset + penetrance)?, hotspot(PM1)-valid locations/patterns, and valid disease variant types (missense only/LOF only/any)
 Once AF cutoffs are decided we should QC by comparing to known pathos and specifically the MVL, plot distribution of AFs for each gene's pathogenic variants</t>
-  </si>
-  <si>
-    <t>get_highest_MAF
-I: VCF variant
-O: highest subpopulation/ethnicity MAF with AC &gt; 2000, only 0% if cov&gt;20x/sample</t>
   </si>
   <si>
     <r>
@@ -341,11 +277,6 @@
     </r>
   </si>
   <si>
-    <t>get_all_population_data
-I: VCF variant
-O: AC, AN, MAF, homo hetero hemiz counts for all available databases and ethnicities/sub-pops</t>
-  </si>
-  <si>
     <t>Supporting display planel /
 Variant browser</t>
   </si>
@@ -437,11 +368,6 @@
 O: five scores from alamut</t>
   </si>
   <si>
-    <t>get_pdot
-I: VCF variant, transcript
-O: HGVS p. (via query of RVS db?)(or run SnpEff?)</t>
-  </si>
-  <si>
     <t>Qatar sequencing study
 (~1000 exomes)</t>
   </si>
@@ -472,9 +398,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>assigned to Dianwei/Sean after clinvar</t>
-  </si>
-  <si>
     <t>Remove duplicates?, lift old transcripts to current, resolve any remaining vkey addition issues, compare to pt VCFs?
 Any work done needs a script to be reran on the most current MVL dump directly preceding VISta usage
 Finalize upload to VISta</t>
@@ -483,6 +406,118 @@
     <t>get_vkey
 I: left-normalized VCF variant
 O: vkey</t>
+  </si>
+  <si>
+    <t>is_pos_covered
+I: chrom, pos
+O: Is the position covered &gt; 20x/sample on average? (yes or no)</t>
+  </si>
+  <si>
+    <t>Done
+(as python script at least, need to add to perl library)</t>
+  </si>
+  <si>
+    <t>This functionality will be provided by Nick from RVS.
+Will import RVS module into VISta library and use his function</t>
+  </si>
+  <si>
+    <t>get_highest_MAF
+I: vkey
+O: highest subpopulation/ethnicity MAF with AN &gt; 2000, only 0% if cov&gt;20x/sample</t>
+  </si>
+  <si>
+    <t>suggest_BS2
+I: chrom, vkey
+O: BS2 or other options</t>
+  </si>
+  <si>
+    <t>get_pdot
+I: vkey, transcript
+O: HGVS p. (via query of RVS)</t>
+  </si>
+  <si>
+    <t>get_variant_type
+I: vkey, transcript
+O: variant type (stopgain, frameshift, CSS, stoploss, startloss, inframe, nonsynonymous, intronic)</t>
+  </si>
+  <si>
+    <t>get_pathogenic_variant_MVL
+I: vkey
+O: Variant info from MVL</t>
+  </si>
+  <si>
+    <t>get_pathogenic_variant
+I: vkey
+O: Variant info from pathogenic dbs with a pathogenic assertion (allow discordant for review purposes)</t>
+  </si>
+  <si>
+    <t>get_pathogenic_variants
+I: chr, start, stop
+O: Potentially multiple variants in the range from pathogenic dbs with a pathogenic assertion (allow discordant for review purposes)</t>
+  </si>
+  <si>
+    <t>get_pathogenic_variants_MVL
+I: chr, start, stop
+O: Potentially multiple variants  in the range from MVL</t>
+  </si>
+  <si>
+    <t>suggest_PS4
+I: vkey, transcript
+O: PS4-M, PS4-P, or other options</t>
+  </si>
+  <si>
+    <t>suggest_BA1_BS1_PM2
+I: chrom, pos, vkey, transcript
+O: BA1, BS1, PM2, or NA if the position is not covered sufficiently</t>
+  </si>
+  <si>
+    <t>suggest_PP5_BP6
+I: vkey
+O: PP5, BP6, or other options (concordant assertions, no publication references, not in MVL, compare get_patho to get_patho_MVL)</t>
+  </si>
+  <si>
+    <t>get_total_genotype_counts
+I: vkey
+O: Total genotype counts at this position (number homoz, hetero, hemiz)</t>
+  </si>
+  <si>
+    <t>get_all_population_data
+I: vkey
+O: AC, AN, MAF, homo hetero hemiz counts for all available databases and ethnicities/sub-pops</t>
+  </si>
+  <si>
+    <t>normalize_VCF_variant
+I: VCF variant
+O: left-normalized VCF variant</t>
+  </si>
+  <si>
+    <t>basically done but not in proj_VISta</t>
+  </si>
+  <si>
+    <t>Manually curated results far off.  Have Gene-transcript from MVL and HGMD</t>
+  </si>
+  <si>
+    <t>Zach's to-do</t>
+  </si>
+  <si>
+    <t>Dianwei to-do</t>
+  </si>
+  <si>
+    <t>dbscSNV</t>
+  </si>
+  <si>
+    <t>rmsk</t>
+  </si>
+  <si>
+    <t>parse and upload to db2</t>
+  </si>
+  <si>
+    <t>Compare, assess, determine cutoffs for REVEL, CADD, metaSVM vs SIFT, PolyPhen2, MutationTaster2
+Consider including VEST3, REVEL, MetaSVM, MutationTaster, Mcap, and CADD (best 6 from Rong email [Plon])</t>
+  </si>
+  <si>
+    <t>basically done but not in proj_VISta
+Dianwei to-do</t>
   </si>
 </sst>
 </file>
@@ -528,7 +563,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,6 +573,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -619,11 +672,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -902,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -921,26 +1019,26 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
@@ -952,16 +1050,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -970,13 +1068,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="14" customFormat="1" ht="80" x14ac:dyDescent="0.2">
@@ -984,16 +1085,16 @@
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D6" s="16">
         <v>3</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>100</v>
+      <c r="E6" s="35" t="s">
+        <v>83</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -1002,15 +1103,17 @@
         <v>0</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D7" s="16">
         <v>3</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="35" t="s">
+        <v>83</v>
+      </c>
       <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" s="14" customFormat="1" ht="96" x14ac:dyDescent="0.2">
@@ -1018,15 +1121,17 @@
         <v>0</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D8" s="16">
         <v>3</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="22" t="s">
+        <v>105</v>
+      </c>
       <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -1034,30 +1139,33 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D9" s="7">
         <v>3</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1065,13 +1173,16 @@
         <v>0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1079,13 +1190,16 @@
         <v>0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1093,532 +1207,576 @@
         <v>0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
       </c>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D14" s="7">
         <v>2</v>
       </c>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="7">
         <v>2</v>
       </c>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="7">
         <v>1</v>
       </c>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="7">
         <v>2</v>
       </c>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
       </c>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="D19" s="7">
         <v>1</v>
       </c>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D20" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>41</v>
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="7"/>
+        <v>109</v>
+      </c>
+      <c r="D21" s="21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="33"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D22" s="7">
         <v>2</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="21">
+        <v>1</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="7">
+        <v>7</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="7">
+        <v>2</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="7">
+        <v>7</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="9" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="13"/>
+      <c r="D28" s="11"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="27">
+        <v>1</v>
+      </c>
+      <c r="E29" s="26"/>
+    </row>
+    <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A30" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="27">
+        <v>1</v>
+      </c>
+      <c r="E30" s="26"/>
+    </row>
+    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A31" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="27">
+        <v>1</v>
+      </c>
+      <c r="E31" s="26"/>
+    </row>
+    <row r="32" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A32" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="27">
+        <v>1</v>
+      </c>
+      <c r="E32" s="26"/>
+    </row>
+    <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A33" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="27">
+        <v>1</v>
+      </c>
+      <c r="E33" s="26"/>
+    </row>
+    <row r="34" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A34" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="31" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="D34" s="32">
+        <v>1</v>
+      </c>
+      <c r="E34" s="30"/>
+    </row>
+    <row r="35" spans="1:6" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="32">
+        <v>1</v>
+      </c>
+      <c r="E35" s="30"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A36" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="32">
+        <v>1</v>
+      </c>
+      <c r="E36" s="30"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A37" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="32">
+        <v>1</v>
+      </c>
+      <c r="E37" s="30"/>
+    </row>
+    <row r="38" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="16">
+        <v>1</v>
+      </c>
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="16">
+        <v>1</v>
+      </c>
+      <c r="E39" s="19"/>
+    </row>
+    <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A40" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D40" s="29">
+        <v>1</v>
+      </c>
+      <c r="E40" s="28"/>
+    </row>
+    <row r="41" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A41" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="29">
+        <v>1</v>
+      </c>
+      <c r="E41" s="28"/>
+    </row>
+    <row r="42" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A42" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="29">
+        <v>1</v>
+      </c>
+      <c r="E42" s="28"/>
+    </row>
+    <row r="43" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" s="9" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="13"/>
-      <c r="D27" s="11"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="3" t="s">
+    <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="C46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="C47" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C48" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="D49" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="D50" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="144" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D43" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D47" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D48" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="C51" s="4" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="D51" s="7">
         <v>1</v>
@@ -1626,13 +1784,13 @@
     </row>
     <row r="52" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="D52" s="7">
         <v>1</v>
@@ -1640,13 +1798,13 @@
     </row>
     <row r="53" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="D53" s="7">
         <v>1</v>
@@ -1654,13 +1812,13 @@
     </row>
     <row r="54" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D54" s="7">
         <v>1</v>
@@ -1668,13 +1826,13 @@
     </row>
     <row r="55" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D55" s="7">
         <v>1</v>
@@ -1682,173 +1840,175 @@
     </row>
     <row r="56" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D56" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="9" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="10"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="11"/>
+    <row r="57" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="D58" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" s="18">
-        <v>1</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="19"/>
+        <v>57</v>
+      </c>
+      <c r="D59" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="9" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="10"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="11"/>
     </row>
     <row r="61" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="19"/>
+        <v>41</v>
+      </c>
+      <c r="D61" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="33">
+        <v>1</v>
+      </c>
+      <c r="E62" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D62" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="B63" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D63" s="7">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="D63" s="33"/>
+      <c r="E63" s="34" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>75</v>
+        <v>36</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D64" s="7">
-        <v>1</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D64" s="33"/>
+      <c r="E64" s="34"/>
     </row>
     <row r="65" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>75</v>
+        <v>36</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="D65" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>75</v>
+        <v>36</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D66" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D67" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D68" s="7">
         <v>1</v>
@@ -1856,68 +2016,101 @@
     </row>
     <row r="69" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B69" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D69" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D70" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D72" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A73" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D69" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D70" s="7">
+      <c r="D73" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D71" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="7">
+    <row r="74" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D74" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D75" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D73" s="7"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D74" s="7"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D75" s="7"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D76" s="7"/>
@@ -1964,11 +2157,17 @@
     <row r="90" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D90" s="7"/>
     </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D91" s="7"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D92" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="E12:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>